<commit_message>
Minor updates to Canada employment data analysis files
Signed-off-by: Brian Krauth <bkrauth@sfu.ca>
</commit_message>
<xml_diff>
--- a/files/CanadaEmploymentHistorical.xlsx
+++ b/files/CanadaEmploymentHistorical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\sfuvault\Professional\website\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BE018F-5182-4487-A3E9-8BBC38047C9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96213F3-8E7D-4136-B09B-E1BD0B8D1F83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1095,9 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>